<commit_message>
illustrative frameworks and gantt correctin
</commit_message>
<xml_diff>
--- a/figures/phd_gantt_chart.xlsx
+++ b/figures/phd_gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA470D65-CDCF-BA47-8BB8-E9C8A6F3E925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41DD583-8107-214D-9B6F-F35B208EDE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="660" windowWidth="38080" windowHeight="20780" activeTab="2" xr2:uid="{BF1E6BC0-DBBC-6047-A9BF-ED803D8A9407}"/>
+    <workbookView xWindow="29580" yWindow="660" windowWidth="38080" windowHeight="20780" activeTab="3" xr2:uid="{BF1E6BC0-DBBC-6047-A9BF-ED803D8A9407}"/>
   </bookViews>
   <sheets>
     <sheet name="Year 1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>Proposal - Litterature review</t>
   </si>
   <si>
-    <t>Paper 1 - Writing</t>
-  </si>
-  <si>
-    <t>Paper 1 - Manuscript submission</t>
-  </si>
-  <si>
     <t>Fall 2024</t>
   </si>
   <si>
@@ -144,69 +138,6 @@
   </si>
   <si>
     <t>Spring-Summer 2028</t>
-  </si>
-  <si>
-    <t>Chapter 1 - Analysis</t>
-  </si>
-  <si>
-    <t>Paper 2 - Manuscript submission</t>
-  </si>
-  <si>
-    <r>
-      <t>Chapter 1 - Writing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (Paper 2)</t>
-    </r>
-  </si>
-  <si>
-    <t>Chapter 2 - Analysis</t>
-  </si>
-  <si>
-    <r>
-      <t>Chapter 2 - Writing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (Paper 3)</t>
-    </r>
-  </si>
-  <si>
-    <t>Paper 3 - Manuscript submission</t>
-  </si>
-  <si>
-    <t>Chapter 3 - Analysis</t>
-  </si>
-  <si>
-    <r>
-      <t>Chapter 3 - Writing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (Paper 4)</t>
-    </r>
-  </si>
-  <si>
-    <t>Paper 4 - Manuscript submission</t>
-  </si>
-  <si>
-    <t>Chapter 4 - Analysis</t>
-  </si>
-  <si>
-    <t>Paper 5 - Manuscript submission</t>
   </si>
   <si>
     <t>Thesis submission</t>
@@ -241,19 +172,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Chapter 4 - Writing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(Paper 5)</t>
-    </r>
-  </si>
-  <si>
     <t>Proposal - Submission</t>
   </si>
   <si>
@@ -283,6 +201,44 @@
   </si>
   <si>
     <t>Conference &amp; Networking</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(TBD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(TBD)</t>
+    </r>
+  </si>
+  <si>
+    <t>Honors student supervision</t>
+  </si>
+  <si>
+    <t>Grants &amp; scholarships application</t>
+  </si>
+  <si>
+    <t>TAC meeting</t>
+  </si>
+  <si>
+    <t>[</t>
   </si>
   <si>
     <r>
@@ -303,12 +259,12 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Finis analysis</t>
+      <t xml:space="preserve"> - Finish analysis</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">TA </t>
+      <t xml:space="preserve">MSc Project </t>
     </r>
     <r>
       <rPr>
@@ -316,12 +272,21 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>(TBD)</t>
+      <t>(Paper 1)</t>
     </r>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Class </t>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Writing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MSc Project </t>
     </r>
     <r>
       <rPr>
@@ -329,20 +294,281 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>(TBD)</t>
+      <t>(Paper 1)</t>
     </r>
-  </si>
-  <si>
-    <t>Honors student supervision</t>
-  </si>
-  <si>
-    <t>Grants &amp; scholarships application</t>
-  </si>
-  <si>
-    <t>TAC meeting</t>
-  </si>
-  <si>
-    <t>[</t>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Manuscript submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">(Paper 2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Writing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Manuscript submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Writing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Manuscript submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Writing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Manuscript submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Writing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chapter 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(Paper 5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Manuscript submission</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -695,18 +921,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -727,10 +945,13 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,19 +960,24 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,148 +1363,148 @@
   <dimension ref="A1:AW34"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="AF20" sqref="AF20"/>
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="90.83203125" customWidth="1"/>
     <col min="2" max="86" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="41"/>
+        <v>6</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="27"/>
     </row>
     <row r="2" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A2" s="38"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35" t="s">
-        <v>12</v>
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="39"/>
+      <c r="R2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="31" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="35" t="s">
-        <v>16</v>
       </c>
       <c r="AE2" s="35"/>
       <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="31" t="s">
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="34" t="s">
         <v>19</v>
-      </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="42" t="s">
-        <v>21</v>
       </c>
       <c r="AU2" s="35"/>
       <c r="AV2" s="35"/>
-      <c r="AW2" s="43"/>
+      <c r="AW2" s="36"/>
     </row>
     <row r="3" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1388,7 +1614,7 @@
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1441,7 +1667,7 @@
     </row>
     <row r="6" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="8"/>
@@ -1494,7 +1720,7 @@
     </row>
     <row r="7" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1598,7 +1824,7 @@
     </row>
     <row r="9" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1651,7 +1877,7 @@
     </row>
     <row r="10" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1760,7 +1986,7 @@
     </row>
     <row r="12" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1866,7 +2092,7 @@
     </row>
     <row r="14" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -1972,7 +2198,7 @@
     </row>
     <row r="16" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2006,16 +2232,16 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="8"/>
       <c r="AG16" s="9"/>
-      <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="7"/>
-      <c r="AL16" s="1"/>
-      <c r="AM16" s="1"/>
+      <c r="AL16" s="8"/>
+      <c r="AM16" s="8"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="7"/>
-      <c r="AP16" s="1"/>
-      <c r="AQ16" s="1"/>
+      <c r="AP16" s="8"/>
+      <c r="AQ16" s="8"/>
       <c r="AR16" s="1"/>
       <c r="AS16" s="7"/>
       <c r="AT16" s="1"/>
@@ -2025,7 +2251,7 @@
     </row>
     <row r="17" spans="1:49" ht="34" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2078,7 +2304,7 @@
     </row>
     <row r="18" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2114,16 +2340,16 @@
       <c r="AG18" s="7"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-      <c r="AK18" s="7"/>
-      <c r="AL18" s="1"/>
-      <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
-      <c r="AO18" s="7"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="50"/>
+      <c r="AM18" s="50"/>
+      <c r="AN18" s="8"/>
+      <c r="AO18" s="9"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
-      <c r="AR18" s="1"/>
-      <c r="AS18" s="7"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="9"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
@@ -2131,7 +2357,7 @@
     </row>
     <row r="19" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2230,7 +2456,7 @@
       <c r="AO20" s="9"/>
       <c r="AP20" s="8"/>
       <c r="AQ20" s="8"/>
-      <c r="AR20" s="50"/>
+      <c r="AR20" s="1"/>
       <c r="AS20" s="7"/>
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
@@ -2292,7 +2518,7 @@
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -2341,17 +2567,17 @@
       <c r="AW22" s="17"/>
     </row>
     <row r="23" spans="1:49" ht="34" x14ac:dyDescent="0.4">
-      <c r="B23" s="27" t="b">
+      <c r="B23" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
@@ -2396,22 +2622,11 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="B1:Q1"/>
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="R1:AG1"/>
@@ -2419,6 +2634,17 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AW2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2431,148 +2657,148 @@
   <dimension ref="A1:AW23"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="90.83203125" customWidth="1"/>
     <col min="2" max="49" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="41"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="27"/>
     </row>
     <row r="2" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A2" s="45"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35" t="s">
-        <v>12</v>
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="39"/>
+      <c r="R2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="31" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="35" t="s">
-        <v>16</v>
       </c>
       <c r="AE2" s="35"/>
       <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="31" t="s">
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="34" t="s">
         <v>19</v>
-      </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="42" t="s">
-        <v>21</v>
       </c>
       <c r="AU2" s="35"/>
       <c r="AV2" s="35"/>
-      <c r="AW2" s="43"/>
+      <c r="AW2" s="36"/>
     </row>
     <row r="3" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -2682,7 +2908,7 @@
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2735,7 +2961,7 @@
     </row>
     <row r="6" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2788,7 +3014,7 @@
     </row>
     <row r="7" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -2841,7 +3067,7 @@
     </row>
     <row r="8" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2894,7 +3120,7 @@
     </row>
     <row r="9" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2998,7 +3224,7 @@
     </row>
     <row r="11" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -3051,7 +3277,7 @@
     </row>
     <row r="12" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A12" s="20" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -3104,7 +3330,7 @@
     </row>
     <row r="13" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A13" s="25" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -3210,7 +3436,7 @@
     </row>
     <row r="15" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -3263,7 +3489,7 @@
     </row>
     <row r="16" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -3316,7 +3542,7 @@
     </row>
     <row r="17" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3350,26 +3576,26 @@
       <c r="AE17" s="8"/>
       <c r="AF17" s="8"/>
       <c r="AG17" s="9"/>
-      <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="7"/>
-      <c r="AL17" s="1"/>
-      <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
-      <c r="AO17" s="7"/>
-      <c r="AP17" s="1"/>
-      <c r="AQ17" s="1"/>
-      <c r="AR17" s="1"/>
-      <c r="AS17" s="7"/>
-      <c r="AT17" s="1"/>
-      <c r="AU17" s="1"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="9"/>
+      <c r="AP17" s="8"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="9"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
       <c r="AV17" s="8"/>
       <c r="AW17" s="2"/>
     </row>
     <row r="18" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -3424,7 +3650,7 @@
     </row>
     <row r="19" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -3583,7 +3809,7 @@
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -3591,20 +3817,25 @@
       <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:49" ht="34" x14ac:dyDescent="0.4">
-      <c r="B23" s="27" t="b">
+      <c r="B23" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -3618,11 +3849,6 @@
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3633,149 +3859,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43554D53-58F0-4749-965A-7E3B076A9C52}">
   <dimension ref="A1:AW23"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView showRowColHeaders="0" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="90.83203125" customWidth="1"/>
     <col min="2" max="49" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="41"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="27"/>
     </row>
     <row r="2" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A2" s="47"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35" t="s">
-        <v>12</v>
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="39"/>
+      <c r="R2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="31" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="35" t="s">
-        <v>16</v>
       </c>
       <c r="AE2" s="35"/>
       <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="31" t="s">
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="34" t="s">
         <v>19</v>
-      </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="42" t="s">
-        <v>21</v>
       </c>
       <c r="AU2" s="35"/>
       <c r="AV2" s="35"/>
-      <c r="AW2" s="43"/>
+      <c r="AW2" s="36"/>
     </row>
     <row r="3" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -3885,7 +4111,7 @@
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -3938,7 +4164,7 @@
     </row>
     <row r="6" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3991,7 +4217,7 @@
     </row>
     <row r="7" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -4044,7 +4270,7 @@
     </row>
     <row r="8" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4097,7 +4323,7 @@
     </row>
     <row r="9" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -4201,7 +4427,7 @@
     </row>
     <row r="11" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -4254,7 +4480,7 @@
     </row>
     <row r="12" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4360,7 +4586,7 @@
     </row>
     <row r="14" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -4413,7 +4639,7 @@
     </row>
     <row r="15" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -4466,7 +4692,7 @@
     </row>
     <row r="16" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -4474,12 +4700,12 @@
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="7"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="1"/>
@@ -4519,7 +4745,7 @@
     </row>
     <row r="17" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4574,7 +4800,7 @@
     </row>
     <row r="18" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4627,7 +4853,7 @@
     </row>
     <row r="19" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4786,7 +5012,7 @@
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -4794,20 +5020,25 @@
       <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:49" ht="34" x14ac:dyDescent="0.4">
-      <c r="B23" s="27" t="b">
+      <c r="B23" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -4821,11 +5052,6 @@
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4836,149 +5062,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC53E47-0772-2045-B234-D1F583413FAE}">
   <dimension ref="A1:AW23"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="90.83203125" customWidth="1"/>
     <col min="2" max="49" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="41"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="27"/>
     </row>
     <row r="2" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A2" s="49"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35" t="s">
-        <v>12</v>
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="39"/>
+      <c r="R2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="31" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="35" t="s">
-        <v>16</v>
       </c>
       <c r="AE2" s="35"/>
       <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="31" t="s">
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="34" t="s">
         <v>19</v>
-      </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="42" t="s">
-        <v>21</v>
       </c>
       <c r="AU2" s="35"/>
       <c r="AV2" s="35"/>
-      <c r="AW2" s="43"/>
+      <c r="AW2" s="36"/>
     </row>
     <row r="3" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -5088,7 +5314,7 @@
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -5141,7 +5367,7 @@
     </row>
     <row r="6" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5194,7 +5420,7 @@
     </row>
     <row r="7" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -5247,7 +5473,7 @@
     </row>
     <row r="8" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5351,7 +5577,7 @@
     </row>
     <row r="10" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -5404,7 +5630,7 @@
     </row>
     <row r="11" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5459,7 +5685,7 @@
     </row>
     <row r="12" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -5513,7 +5739,7 @@
     </row>
     <row r="13" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5619,7 +5845,7 @@
     </row>
     <row r="15" spans="1:49" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -5672,7 +5898,7 @@
     </row>
     <row r="16" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B16" s="16" t="b">
         <v>1</v>
@@ -5727,7 +5953,7 @@
     </row>
     <row r="17" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -5780,7 +6006,7 @@
     </row>
     <row r="18" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5833,7 +6059,7 @@
     </row>
     <row r="19" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5888,7 +6114,7 @@
     </row>
     <row r="20" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -5994,7 +6220,7 @@
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -6002,20 +6228,25 @@
       <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:49" ht="34" x14ac:dyDescent="0.4">
-      <c r="B23" s="27" t="b">
+      <c r="B23" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -6029,11 +6260,6 @@
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>